<commit_message>
D13 placement, R76 value changed, D21 removed
</commit_message>
<xml_diff>
--- a/SOURCES/kiCAD/JLPCB_Oder files (DIFF and BAL)/FreeDSP_OCTAVIA_BOM1.xlsx
+++ b/SOURCES/kiCAD/JLPCB_Oder files (DIFF and BAL)/FreeDSP_OCTAVIA_BOM1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/FreeDSP-OCTAVIA/FreeDSP_OCTAVIA/SOURCES/kiCAD/JLPCB_Oder files (DIFF and BAL)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A7B3E5-4EE3-2642-AD62-76DA4B0073CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2200F677-E2D0-FB44-994F-3786299DB51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="7120" windowWidth="40140" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="603">
   <si>
     <t xml:space="preserve">    C3</t>
   </si>
@@ -1048,9 +1048,6 @@
   </si>
   <si>
     <t xml:space="preserve">    D12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    D13</t>
   </si>
   <si>
     <t xml:space="preserve">    D14</t>
@@ -1893,6 +1890,10 @@
   </si>
   <si>
     <t>C86715</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>330R</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2287,11 +2288,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D422"/>
+  <dimension ref="A1:D421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D410" sqref="D410"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A165" sqref="A165:XFD165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2304,16 +2305,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>578</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2321,7 +2322,7 @@
         <v>98</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>99</v>
@@ -2335,7 +2336,7 @@
         <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>99</v>
@@ -2349,7 +2350,7 @@
         <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>99</v>
@@ -2363,7 +2364,7 @@
         <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>116</v>
@@ -2377,13 +2378,13 @@
         <v>112</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2391,13 +2392,13 @@
         <v>140</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2405,13 +2406,13 @@
         <v>153</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2419,7 +2420,7 @@
         <v>156</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>116</v>
@@ -2433,13 +2434,13 @@
         <v>115</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2447,13 +2448,13 @@
         <v>115</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2461,13 +2462,13 @@
         <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2475,13 +2476,13 @@
         <v>115</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2489,13 +2490,13 @@
         <v>115</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2503,13 +2504,13 @@
         <v>115</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2517,13 +2518,13 @@
         <v>115</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2531,13 +2532,13 @@
         <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2545,7 +2546,7 @@
         <v>156</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>116</v>
@@ -2559,7 +2560,7 @@
         <v>156</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>116</v>
@@ -2573,13 +2574,13 @@
         <v>115</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2587,7 +2588,7 @@
         <v>156</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>116</v>
@@ -2601,13 +2602,13 @@
         <v>185</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>184</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2615,13 +2616,13 @@
         <v>185</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>184</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2632,7 +2633,7 @@
         <v>196</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>198</v>
@@ -4600,156 +4601,156 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="3" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>337</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>338</v>
+        <v>52</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>52</v>
+        <v>338</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>339</v>
+        <v>59</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>65</v>
+        <v>327</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>327</v>
+        <v>68</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="3" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>68</v>
+        <v>339</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>340</v>
+        <v>46</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>46</v>
+        <v>328</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4757,7 +4758,7 @@
         <v>43</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>44</v>
@@ -4771,7 +4772,7 @@
         <v>43</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>44</v>
@@ -4785,7 +4786,7 @@
         <v>43</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>44</v>
@@ -4799,7 +4800,7 @@
         <v>43</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>44</v>
@@ -4810,41 +4811,41 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="3" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>73</v>
@@ -4880,13 +4881,13 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>351</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>73</v>
@@ -4894,13 +4895,13 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>352</v>
+        <v>70</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>73</v>
@@ -4908,16 +4909,16 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>70</v>
+        <v>341</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4936,16 +4937,16 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>343</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -5006,80 +5007,80 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>348</v>
+        <v>80</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>80</v>
+        <v>352</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>353</v>
+        <v>87</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>85</v>
+        <v>597</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>598</v>
+        <v>77</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>90</v>
+        <v>353</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>354</v>
+        <v>96</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>94</v>
@@ -5090,10 +5091,10 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>96</v>
+        <v>354</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>94</v>
@@ -5118,30 +5119,30 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>356</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="3" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -5160,30 +5161,30 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>367</v>
+        <v>105</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>105</v>
+        <v>367</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -5202,16 +5203,16 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>369</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -5272,30 +5273,30 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>358</v>
+        <v>374</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -5412,21 +5413,21 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>359</v>
@@ -5435,12 +5436,12 @@
         <v>99</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>360</v>
@@ -5449,12 +5450,12 @@
         <v>99</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>361</v>
@@ -5463,12 +5464,12 @@
         <v>99</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>362</v>
@@ -5477,12 +5478,12 @@
         <v>99</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>363</v>
@@ -5491,7 +5492,7 @@
         <v>99</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5510,16 +5511,16 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" s="3" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>365</v>
+        <v>453</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5566,7 +5567,7 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" s="3" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>457</v>
@@ -5575,7 +5576,7 @@
         <v>113</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>145</v>
+        <v>575</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5589,7 +5590,7 @@
         <v>113</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5603,7 +5604,7 @@
         <v>113</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5617,12 +5618,12 @@
         <v>113</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>461</v>
@@ -5631,35 +5632,35 @@
         <v>113</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>576</v>
+        <v>114</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>462</v>
+        <v>391</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="3" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>392</v>
+        <v>463</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5790,30 +5791,30 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" s="3" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>473</v>
+        <v>392</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" s="3" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>393</v>
+        <v>473</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5832,7 +5833,7 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" s="3" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>475</v>
@@ -5841,7 +5842,7 @@
         <v>116</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5944,49 +5945,49 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="3" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>483</v>
+        <v>119</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" s="3" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="263" spans="1:4">
       <c r="A263" s="3" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>161</v>
+        <v>483</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" s="3" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>484</v>
@@ -5995,7 +5996,7 @@
         <v>116</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -6098,30 +6099,30 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" s="3" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>492</v>
+        <v>393</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" s="3" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>394</v>
+        <v>492</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -6210,35 +6211,35 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="3" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>499</v>
+        <v>124</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="3" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>124</v>
+        <v>499</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>500</v>
@@ -6247,7 +6248,7 @@
         <v>116</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -6294,16 +6295,16 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>504</v>
       </c>
       <c r="C286" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -6322,16 +6323,16 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>506</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -6364,44 +6365,44 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>509</v>
+        <v>394</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D291" s="3" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="3" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>395</v>
+        <v>509</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D292" s="3" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B293" s="3" t="s">
         <v>510</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D293" s="3" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -6420,7 +6421,7 @@
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="3" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B295" s="3" t="s">
         <v>512</v>
@@ -6429,7 +6430,7 @@
         <v>113</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -6518,35 +6519,35 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="3" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>519</v>
+        <v>395</v>
       </c>
       <c r="C302" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D302" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>396</v>
+        <v>519</v>
       </c>
       <c r="C303" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D303" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="3" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="B304" s="3" t="s">
         <v>520</v>
@@ -6555,7 +6556,7 @@
         <v>113</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -6574,16 +6575,16 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>522</v>
       </c>
       <c r="C306" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D306" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6672,30 +6673,30 @@
     </row>
     <row r="313" spans="1:4">
       <c r="A313" s="3" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>529</v>
+        <v>396</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D313" s="3" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
     </row>
     <row r="314" spans="1:4">
       <c r="A314" s="3" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>397</v>
+        <v>529</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D314" s="3" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -6784,30 +6785,30 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="3" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>536</v>
+        <v>397</v>
       </c>
       <c r="C321" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D321" s="3" t="s">
-        <v>152</v>
+        <v>575</v>
       </c>
     </row>
     <row r="322" spans="1:4">
       <c r="A322" s="3" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>398</v>
+        <v>536</v>
       </c>
       <c r="C322" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D322" s="3" t="s">
-        <v>576</v>
+        <v>152</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -6826,7 +6827,7 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>538</v>
@@ -6835,7 +6836,7 @@
         <v>116</v>
       </c>
       <c r="D324" s="3" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -6882,16 +6883,16 @@
     </row>
     <row r="328" spans="1:4">
       <c r="A328" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B328" s="3" t="s">
         <v>542</v>
       </c>
       <c r="C328" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D328" s="3" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6910,16 +6911,16 @@
     </row>
     <row r="330" spans="1:4">
       <c r="A330" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B330" s="3" t="s">
         <v>544</v>
       </c>
       <c r="C330" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D330" s="3" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -6938,44 +6939,44 @@
     </row>
     <row r="332" spans="1:4">
       <c r="A332" s="3" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>546</v>
+        <v>384</v>
       </c>
       <c r="C332" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D332" s="3" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D333" s="3" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="334" spans="1:4">
       <c r="A334" s="3" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>399</v>
+        <v>546</v>
       </c>
       <c r="C334" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D334" s="3" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -6994,21 +6995,21 @@
     </row>
     <row r="336" spans="1:4">
       <c r="A336" s="3" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B336" s="3" t="s">
         <v>548</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D336" s="3" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
     </row>
     <row r="337" spans="1:4">
       <c r="A337" s="3" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B337" s="3" t="s">
         <v>549</v>
@@ -7017,7 +7018,7 @@
         <v>113</v>
       </c>
       <c r="D337" s="3" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -7036,7 +7037,7 @@
     </row>
     <row r="339" spans="1:4">
       <c r="A339" s="3" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B339" s="3" t="s">
         <v>551</v>
@@ -7045,7 +7046,7 @@
         <v>113</v>
       </c>
       <c r="D339" s="3" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -7106,30 +7107,30 @@
     </row>
     <row r="344" spans="1:4">
       <c r="A344" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>556</v>
+        <v>399</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D344" s="3" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="345" spans="1:4">
       <c r="A345" s="3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>400</v>
+        <v>556</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D345" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -7148,7 +7149,7 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" s="3" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="B347" s="3" t="s">
         <v>558</v>
@@ -7157,7 +7158,7 @@
         <v>113</v>
       </c>
       <c r="D347" s="3" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -7176,21 +7177,21 @@
     </row>
     <row r="349" spans="1:4">
       <c r="A349" s="3" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>560</v>
+        <v>400</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D349" s="3" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="350" spans="1:4">
       <c r="A350" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B350" s="3" t="s">
         <v>401</v>
@@ -7199,12 +7200,12 @@
         <v>113</v>
       </c>
       <c r="D350" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B351" s="3" t="s">
         <v>402</v>
@@ -7213,7 +7214,7 @@
         <v>113</v>
       </c>
       <c r="D351" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -7232,7 +7233,7 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B353" s="3" t="s">
         <v>404</v>
@@ -7241,7 +7242,7 @@
         <v>113</v>
       </c>
       <c r="D353" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -7260,35 +7261,35 @@
     </row>
     <row r="355" spans="1:4">
       <c r="A355" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>406</v>
+        <v>135</v>
       </c>
       <c r="C355" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D355" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="356" spans="1:4">
       <c r="A356" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>135</v>
+        <v>409</v>
       </c>
       <c r="C356" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D356" s="3" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
     </row>
     <row r="357" spans="1:4">
       <c r="A357" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B357" s="3" t="s">
         <v>410</v>
@@ -7297,12 +7298,12 @@
         <v>113</v>
       </c>
       <c r="D357" s="3" t="s">
-        <v>114</v>
+        <v>575</v>
       </c>
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>411</v>
@@ -7311,12 +7312,12 @@
         <v>113</v>
       </c>
       <c r="D358" s="3" t="s">
-        <v>576</v>
+        <v>114</v>
       </c>
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>412</v>
@@ -7325,7 +7326,7 @@
         <v>113</v>
       </c>
       <c r="D359" s="3" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -7358,16 +7359,16 @@
     </row>
     <row r="362" spans="1:4">
       <c r="A362" s="3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>415</v>
       </c>
       <c r="C362" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D362" s="3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -7375,7 +7376,7 @@
         <v>138</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>116</v>
@@ -7386,21 +7387,21 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B364" s="3" t="s">
         <v>418</v>
       </c>
       <c r="C364" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D364" s="3" t="s">
-        <v>139</v>
+        <v>575</v>
       </c>
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="B365" s="3" t="s">
         <v>419</v>
@@ -7409,40 +7410,40 @@
         <v>113</v>
       </c>
       <c r="D365" s="3" t="s">
-        <v>576</v>
+        <v>141</v>
       </c>
     </row>
     <row r="366" spans="1:4">
       <c r="A366" s="3" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C366" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D366" s="3" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="367" spans="1:4">
       <c r="A367" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>422</v>
+        <v>387</v>
       </c>
       <c r="C367" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D367" s="3" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
     </row>
     <row r="368" spans="1:4">
       <c r="A368" s="3" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="B368" s="3" t="s">
         <v>388</v>
@@ -7451,26 +7452,26 @@
         <v>113</v>
       </c>
       <c r="D368" s="3" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="3" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>389</v>
+        <v>422</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D369" s="3" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
     </row>
     <row r="370" spans="1:4">
       <c r="A370" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B370" s="3" t="s">
         <v>423</v>
@@ -7479,96 +7480,96 @@
         <v>113</v>
       </c>
       <c r="D370" s="3" t="s">
-        <v>114</v>
+        <v>575</v>
       </c>
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="3" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D371" s="3" t="s">
-        <v>576</v>
+        <v>143</v>
       </c>
     </row>
     <row r="372" spans="1:4">
       <c r="A372" s="3" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>427</v>
+        <v>389</v>
       </c>
       <c r="C372" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D372" s="3" t="s">
-        <v>143</v>
+        <v>575</v>
       </c>
     </row>
     <row r="373" spans="1:4">
       <c r="A373" s="3" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D373" s="3" t="s">
-        <v>576</v>
+        <v>145</v>
       </c>
     </row>
     <row r="374" spans="1:4">
       <c r="A374" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>428</v>
+        <v>146</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D374" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="375" spans="1:4">
       <c r="A375" s="3" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C375" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D375" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="376" spans="1:4">
       <c r="A376" s="3" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>149</v>
+        <v>428</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D376" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="377" spans="1:4">
       <c r="A377" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B377" s="3" t="s">
         <v>429</v>
@@ -7577,12 +7578,12 @@
         <v>116</v>
       </c>
       <c r="D377" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="378" spans="1:4">
       <c r="A378" s="3" t="s">
-        <v>142</v>
+        <v>602</v>
       </c>
       <c r="B378" s="3" t="s">
         <v>430</v>
@@ -7591,12 +7592,12 @@
         <v>116</v>
       </c>
       <c r="D378" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="379" spans="1:4">
       <c r="A379" s="3" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B379" s="3" t="s">
         <v>431</v>
@@ -7605,7 +7606,7 @@
         <v>116</v>
       </c>
       <c r="D379" s="3" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7638,30 +7639,30 @@
     </row>
     <row r="382" spans="1:4">
       <c r="A382" s="3" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>434</v>
+        <v>390</v>
       </c>
       <c r="C382" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D382" s="3" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="3" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="C383" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D383" s="3" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -7708,7 +7709,7 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="3" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="B387" s="3" t="s">
         <v>438</v>
@@ -7717,12 +7718,12 @@
         <v>116</v>
       </c>
       <c r="D387" s="3" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
     </row>
     <row r="388" spans="1:4">
       <c r="A388" s="3" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="B388" s="3" t="s">
         <v>439</v>
@@ -7731,35 +7732,35 @@
         <v>116</v>
       </c>
       <c r="D388" s="3" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="389" spans="1:4">
       <c r="A389" s="3" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>440</v>
+        <v>155</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D389" s="3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="390" spans="1:4">
       <c r="A390" s="3" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>155</v>
+        <v>441</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D390" s="3" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -7791,22 +7792,22 @@
       </c>
     </row>
     <row r="393" spans="1:4">
-      <c r="A393" s="3" t="s">
-        <v>138</v>
+      <c r="A393" s="3">
+        <v>100</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C393" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D393" s="3" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="394" spans="1:4">
-      <c r="A394" s="3">
-        <v>100</v>
+      <c r="A394" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="B394" s="3" t="s">
         <v>446</v>
@@ -7815,12 +7816,12 @@
         <v>113</v>
       </c>
       <c r="D394" s="3" t="s">
-        <v>158</v>
+        <v>575</v>
       </c>
     </row>
     <row r="395" spans="1:4">
-      <c r="A395" s="3" t="s">
-        <v>118</v>
+      <c r="A395" s="3">
+        <v>100</v>
       </c>
       <c r="B395" s="3" t="s">
         <v>447</v>
@@ -7829,63 +7830,63 @@
         <v>113</v>
       </c>
       <c r="D395" s="3" t="s">
-        <v>576</v>
+        <v>158</v>
       </c>
     </row>
     <row r="396" spans="1:4">
-      <c r="A396" s="3">
-        <v>100</v>
+      <c r="A396" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="B396" s="3" t="s">
         <v>448</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D396" s="3" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="397" spans="1:4">
       <c r="A397" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B397" s="3" t="s">
         <v>449</v>
       </c>
       <c r="C397" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D397" s="3" t="s">
-        <v>139</v>
+        <v>575</v>
       </c>
     </row>
     <row r="398" spans="1:4">
       <c r="A398" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B398" s="3" t="s">
         <v>450</v>
       </c>
       <c r="C398" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D398" s="3" t="s">
-        <v>576</v>
+        <v>164</v>
       </c>
     </row>
     <row r="399" spans="1:4">
       <c r="A399" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B399" s="3" t="s">
         <v>451</v>
       </c>
       <c r="C399" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D399" s="3" t="s">
-        <v>164</v>
+        <v>575</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -7899,63 +7900,63 @@
         <v>113</v>
       </c>
       <c r="D400" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="401" spans="1:4">
       <c r="A401" s="3" t="s">
-        <v>118</v>
+        <v>183</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>453</v>
+        <v>182</v>
       </c>
       <c r="C401" s="3" t="s">
-        <v>113</v>
+        <v>184</v>
       </c>
       <c r="D401" s="3" t="s">
-        <v>576</v>
+        <v>595</v>
       </c>
     </row>
     <row r="402" spans="1:4">
       <c r="A402" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C402" s="3" t="s">
-        <v>184</v>
+        <v>598</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>596</v>
+        <v>188</v>
       </c>
     </row>
     <row r="403" spans="1:4">
       <c r="A403" s="3" t="s">
-        <v>187</v>
+        <v>599</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C403" s="3" t="s">
-        <v>599</v>
+        <v>190</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>188</v>
+        <v>600</v>
       </c>
     </row>
     <row r="404" spans="1:4">
       <c r="A404" s="3" t="s">
-        <v>600</v>
+        <v>191</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>189</v>
+        <v>562</v>
       </c>
       <c r="C404" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>601</v>
+        <v>193</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -7963,7 +7964,7 @@
         <v>191</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C405" s="3" t="s">
         <v>192</v>
@@ -8002,16 +8003,16 @@
     </row>
     <row r="408" spans="1:4">
       <c r="A408" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B408" s="3" t="s">
         <v>567</v>
       </c>
       <c r="C408" s="3" t="s">
-        <v>192</v>
+        <v>596</v>
       </c>
       <c r="D408" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -8022,10 +8023,10 @@
         <v>568</v>
       </c>
       <c r="C409" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D409" s="3" t="s">
-        <v>195</v>
+        <v>601</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -8036,10 +8037,10 @@
         <v>569</v>
       </c>
       <c r="C410" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D410" s="3" t="s">
-        <v>602</v>
+        <v>195</v>
       </c>
     </row>
     <row r="411" spans="1:4">
@@ -8050,7 +8051,7 @@
         <v>570</v>
       </c>
       <c r="C411" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D411" s="3" t="s">
         <v>195</v>
@@ -8064,7 +8065,7 @@
         <v>571</v>
       </c>
       <c r="C412" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D412" s="3" t="s">
         <v>195</v>
@@ -8078,7 +8079,7 @@
         <v>572</v>
       </c>
       <c r="C413" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D413" s="3" t="s">
         <v>195</v>
@@ -8092,7 +8093,7 @@
         <v>573</v>
       </c>
       <c r="C414" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D414" s="3" t="s">
         <v>195</v>
@@ -8106,7 +8107,7 @@
         <v>574</v>
       </c>
       <c r="C415" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D415" s="3" t="s">
         <v>195</v>
@@ -8114,93 +8115,79 @@
     </row>
     <row r="416" spans="1:4">
       <c r="A416" s="3" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>575</v>
+        <v>167</v>
       </c>
       <c r="C416" s="3" t="s">
-        <v>597</v>
+        <v>169</v>
       </c>
       <c r="D416" s="3" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
     </row>
     <row r="417" spans="1:4">
       <c r="A417" s="3" t="s">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>167</v>
+        <v>560</v>
       </c>
       <c r="C417" s="3" t="s">
-        <v>169</v>
+        <v>85</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
     </row>
     <row r="418" spans="1:4">
       <c r="A418" s="3" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>561</v>
+        <v>171</v>
       </c>
       <c r="C418" s="3" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="D418" s="3" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
     </row>
     <row r="419" spans="1:4">
       <c r="A419" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C419" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D419" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="420" spans="1:4">
       <c r="A420" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C420" s="3" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D420" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="421" spans="1:4">
-      <c r="A421" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B421" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C421" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D421" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="422" spans="1:4">
-      <c r="A422" s="3"/>
-      <c r="B422" s="2"/>
-      <c r="C422" s="3"/>
-      <c r="D422" s="3"/>
+      <c r="A421" s="3"/>
+      <c r="B421" s="2"/>
+      <c r="C421" s="3"/>
+      <c r="D421" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>